<commit_message>
Strongly signed the assembly Fixed issues 7065, 7064
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/SheetProtection.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/SheetProtection.xlsx
@@ -513,7 +513,7 @@
       <x:c r="B4" s="10" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:sheetProtection sheet="1"/>
+  <x:sheetProtection sheet="1" formatCells="0" insertColumns="0" deleteColumns="0" deleteRows="0"/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
@@ -540,7 +540,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData/>
-  <x:sheetProtection password="CF7A" sheet="1"/>
+  <x:sheetProtection password="CF7A" sheet="1" insertColumns="0" insertRows="0"/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>